<commit_message>
Commit 4: Fixed db errors
</commit_message>
<xml_diff>
--- a/SuperSonic Burndown.xlsx
+++ b/SuperSonic Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\University\Information Technology\IFB299\IFB299-Super-Sonic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3AEFE39B-9AA8-41A2-8FFF-1C76AF9E1080}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1CD71E21-D890-4CAE-8229-95C9D8BAA422}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="462" windowWidth="33600" windowHeight="20520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -106,7 +106,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -114,11 +114,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -131,6 +146,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,8 +556,35 @@
                 <c:pt idx="0">
                   <c:v>26</c:v>
                 </c:pt>
+                <c:pt idx="1">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22</c:v>
+                </c:pt>
                 <c:pt idx="5">
                   <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1002,10 +1052,17 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>'Burn down chart'!$A$3:$A$7</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Burn down chart'!$A$3:$A$7</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Burn down chart'!$A$3:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1017,19 +1074,23 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burn down chart'!$B$3:$B$7</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Burn down chart'!$B$3:$B$7</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Burn down chart'!$B$3:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>70</c:v>
                 </c:pt>
@@ -1040,9 +1101,6 @@
                   <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1095,10 +1153,17 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Burn down chart'!$A$3:$A$7</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Burn down chart'!$A$3:$A$7</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Burn down chart'!$A$3:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1110,15 +1175,19 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Burn down chart'!$C$3:$C$5</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
               <c:f>'Burn down chart'!$C$3:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -4179,234 +4248,296 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G117"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.83203125" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="16384" width="29.83203125" style="1"/>
+    <col min="1" max="1" width="19.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.38671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="29.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="14.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A3" s="1">
+      <c r="A3" s="7">
         <v>0</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="7">
         <v>70</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="7">
         <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A4" s="1">
+      <c r="A4" s="7">
         <v>1</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="7">
         <v>58</v>
       </c>
+      <c r="C4" s="7"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A5" s="1">
+      <c r="A5" s="7">
         <v>2</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="7">
         <v>26</v>
       </c>
+      <c r="C5" s="7"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A6" s="1">
+      <c r="A6" s="7">
         <v>3</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="7">
         <v>0</v>
       </c>
+      <c r="C6" s="7"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A7" s="1">
-        <v>4</v>
-      </c>
-      <c r="B7" s="1">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A11" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A12" s="7" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A11" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="7" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A13" s="1">
+      <c r="A13" s="7">
         <v>20</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="7">
         <v>26</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="7">
         <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A14" s="1">
+      <c r="A14" s="7">
         <v>19</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7">
+        <v>26</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A15" s="1">
+      <c r="A15" s="7">
         <v>18</v>
       </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7">
+        <v>24</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A16" s="1">
+      <c r="A16" s="7">
         <v>17</v>
       </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7">
+        <v>22</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A17" s="1">
+      <c r="A17" s="7">
         <v>16</v>
       </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7">
+        <v>22</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A18" s="1">
+      <c r="A18" s="7">
         <v>15</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="7">
         <v>20</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="7">
         <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A19" s="1">
+      <c r="A19" s="7">
         <v>14</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7">
+        <v>20</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A20" s="1">
+      <c r="A20" s="7">
         <v>13</v>
       </c>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7">
+        <v>20</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A21" s="1">
+      <c r="A21" s="7">
         <v>12</v>
       </c>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7">
+        <v>14</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A22" s="1">
+      <c r="A22" s="7">
         <v>11</v>
       </c>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7">
+        <v>8</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A23" s="1">
+      <c r="A23" s="7">
         <v>10</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="7">
         <v>15</v>
       </c>
+      <c r="C23" s="7">
+        <v>8</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A24" s="1">
+      <c r="A24" s="7">
         <v>9</v>
       </c>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
       <c r="D24" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A25" s="1">
+      <c r="A25" s="7">
         <v>8</v>
       </c>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A26" s="1">
+      <c r="A26" s="7">
         <v>7</v>
       </c>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A27" s="1">
+      <c r="A27" s="7">
         <v>6</v>
       </c>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A28" s="1">
+      <c r="A28" s="7">
         <v>5</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="7">
         <v>10</v>
       </c>
+      <c r="C28" s="7"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A29" s="1">
+      <c r="A29" s="7">
         <v>4</v>
       </c>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
       <c r="D29" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A30" s="1">
+      <c r="A30" s="7">
         <v>3</v>
       </c>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A31" s="1">
+      <c r="A31" s="7">
         <v>2</v>
       </c>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A32" s="1">
+      <c r="A32" s="7">
         <v>1</v>
       </c>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
       <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A33" s="1">
+      <c r="A33" s="7">
         <v>0</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33" s="7">
         <v>0</v>
       </c>
+      <c r="C33" s="7"/>
       <c r="D33" s="2"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
Commit 5: Started to add html to urls
</commit_message>
<xml_diff>
--- a/SuperSonic Burndown.xlsx
+++ b/SuperSonic Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\University\Information Technology\IFB299\IFB299-Super-Sonic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1CD71E21-D890-4CAE-8229-95C9D8BAA422}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{794A392C-FF3F-4A30-91BB-AC78F00845A6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="462" windowWidth="33600" windowHeight="20520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -137,23 +137,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -549,10 +549,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burn down chart'!$C$13:$C$25</c:f>
+              <c:f>'Burn down chart'!$C$13:$C$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>26</c:v>
                 </c:pt>
@@ -585,6 +585,21 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4249,7 +4264,7 @@
   <dimension ref="A1:G117"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.83203125" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -4262,72 +4277,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="14.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A3" s="7">
+      <c r="A3" s="3">
         <v>0</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="3">
         <v>70</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="3">
         <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A4" s="7">
+      <c r="A4" s="3">
         <v>1</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="3">
         <v>58</v>
       </c>
-      <c r="C4" s="7"/>
+      <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A5" s="7">
+      <c r="A5" s="3">
         <v>2</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="3">
         <v>26</v>
       </c>
-      <c r="C5" s="7"/>
+      <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A6" s="7">
+      <c r="A6" s="3">
         <v>3</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="3">
         <v>0</v>
       </c>
-      <c r="C6" s="7"/>
+      <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" s="8" t="s">
@@ -4337,33 +4352,33 @@
       <c r="C11" s="8"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A13" s="7">
+      <c r="A13" s="3">
         <v>20</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="3">
         <v>26</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="3">
         <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A14" s="7">
+      <c r="A14" s="3">
         <v>19</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3">
         <v>26</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -4371,49 +4386,49 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A15" s="7">
+      <c r="A15" s="3">
         <v>18</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3">
         <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A16" s="7">
+      <c r="A16" s="3">
         <v>17</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3">
         <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A17" s="7">
+      <c r="A17" s="3">
         <v>16</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3">
         <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A18" s="7">
+      <c r="A18" s="3">
         <v>15</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" s="3">
         <v>20</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="3">
         <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A19" s="7">
+      <c r="A19" s="3">
         <v>14</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3">
         <v>20</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -4421,134 +4436,144 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A20" s="7">
+      <c r="A20" s="3">
         <v>13</v>
       </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7">
+      <c r="B20" s="3"/>
+      <c r="C20" s="3">
         <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A21" s="7">
+      <c r="A21" s="3">
         <v>12</v>
       </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7">
+      <c r="B21" s="3"/>
+      <c r="C21" s="3">
         <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A22" s="7">
+      <c r="A22" s="3">
         <v>11</v>
       </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7">
+      <c r="B22" s="3"/>
+      <c r="C22" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A23" s="7">
+      <c r="A23" s="3">
         <v>10</v>
       </c>
-      <c r="B23" s="7">
+      <c r="B23" s="3">
         <v>15</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A24" s="7">
+      <c r="A24" s="3">
         <v>9</v>
       </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3">
+        <v>8</v>
+      </c>
       <c r="D24" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A25" s="7">
+      <c r="A25" s="3">
         <v>8</v>
       </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3">
+        <v>8</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A26" s="7">
+      <c r="A26" s="3">
         <v>7</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3">
+        <v>8</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A27" s="7">
+      <c r="A27" s="3">
         <v>6</v>
       </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3">
+        <v>6</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A28" s="7">
+      <c r="A28" s="3">
         <v>5</v>
       </c>
-      <c r="B28" s="7">
+      <c r="B28" s="3">
         <v>10</v>
       </c>
-      <c r="C28" s="7"/>
+      <c r="C28" s="3">
+        <v>6</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A29" s="7">
+      <c r="A29" s="3">
         <v>4</v>
       </c>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
       <c r="D29" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A30" s="7">
+      <c r="A30" s="3">
         <v>3</v>
       </c>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A31" s="7">
+      <c r="A31" s="3">
         <v>2</v>
       </c>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A32" s="7">
+      <c r="A32" s="3">
         <v>1</v>
       </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
       <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A33" s="7">
+      <c r="A33" s="3">
         <v>0</v>
       </c>
-      <c r="B33" s="7">
+      <c r="B33" s="3">
         <v>0</v>
       </c>
-      <c r="C33" s="7"/>
+      <c r="C33" s="3"/>
       <c r="D33" s="2"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.4">
       <c r="D35" s="2"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A37" s="1" t="s">
@@ -4684,9 +4709,9 @@
       <c r="D58" s="2"/>
     </row>
     <row r="64" spans="1:4" ht="14.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A64" s="3"/>
-      <c r="B64" s="4"/>
-      <c r="C64" s="4"/>
+      <c r="A64" s="6"/>
+      <c r="B64" s="7"/>
+      <c r="C64" s="7"/>
     </row>
     <row r="66" spans="4:4" x14ac:dyDescent="0.4">
       <c r="D66" s="2"/>
@@ -4734,9 +4759,9 @@
       <c r="D80" s="2"/>
     </row>
     <row r="101" spans="1:4" ht="14.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A101" s="3"/>
-      <c r="B101" s="4"/>
-      <c r="C101" s="4"/>
+      <c r="A101" s="6"/>
+      <c r="B101" s="7"/>
+      <c r="C101" s="7"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.4">
       <c r="D103" s="2"/>

</xml_diff>

<commit_message>
Commit 8: Cleaned up and set up with html blocks
</commit_message>
<xml_diff>
--- a/SuperSonic Burndown.xlsx
+++ b/SuperSonic Burndown.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\University\Information Technology\IFB299\IFB299-Super-Sonic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarry\OneDrive\Documents\University\Information Technology\IFB299\IFB299-Super-Sonic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{794A392C-FF3F-4A30-91BB-AC78F00845A6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7FCAAF57-6CFA-4692-A296-9140539A22C3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="462" windowWidth="33600" windowHeight="20520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>Sprint Days Remaining</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>Week  Monday</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -599,6 +602,21 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="15">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -1208,7 +1226,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>70</c:v>
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>63</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4264,7 +4285,7 @@
   <dimension ref="A1:G117"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.83203125" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -4304,7 +4325,7 @@
         <v>70</v>
       </c>
       <c r="C3" s="3">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
@@ -4314,7 +4335,9 @@
       <c r="B4" s="3">
         <v>58</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="3">
+        <v>63</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="3">
@@ -4528,7 +4551,9 @@
         <v>4</v>
       </c>
       <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
+      <c r="C29" s="3">
+        <v>6</v>
+      </c>
       <c r="D29" s="1" t="s">
         <v>11</v>
       </c>
@@ -4538,21 +4563,27 @@
         <v>3</v>
       </c>
       <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
+      <c r="C30" s="3">
+        <v>6</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A31" s="3">
         <v>2</v>
       </c>
       <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
+      <c r="C31" s="3">
+        <v>6</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A32" s="3">
         <v>1</v>
       </c>
       <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
+      <c r="C32" s="3">
+        <v>6</v>
+      </c>
       <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.4">
@@ -4562,8 +4593,15 @@
       <c r="B33" s="3">
         <v>0</v>
       </c>
-      <c r="C33" s="3"/>
+      <c r="C33" s="3">
+        <v>6</v>
+      </c>
       <c r="D33" s="2"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C34" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.4">
       <c r="D35" s="2"/>

</xml_diff>

<commit_message>
Commit 10: Small changes, html images not showing and css missing only with django
</commit_message>
<xml_diff>
--- a/SuperSonic Burndown.xlsx
+++ b/SuperSonic Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarry\OneDrive\Documents\University\Information Technology\IFB299\IFB299-Super-Sonic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7FCAAF57-6CFA-4692-A296-9140539A22C3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{38F3161B-BDE2-4F9A-9672-704EC64A16F4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="462" windowWidth="33600" windowHeight="20520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Sprint Days Remaining</t>
   </si>
@@ -69,10 +69,19 @@
     <t>Sprint 2 Burndown</t>
   </si>
   <si>
-    <t>Week  Monday</t>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>Week 10 Monday</t>
+  </si>
+  <si>
+    <t>Week 12 Monday</t>
+  </si>
+  <si>
+    <t>Week 11 Monday</t>
+  </si>
+  <si>
+    <t>Week 13 Monday</t>
   </si>
 </sst>
 </file>
@@ -1226,7 +1235,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>63</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>63</c:v>
@@ -1771,6 +1780,18 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5</c:v>
+                </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1896,10 +1917,58 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burn down chart'!$C$38:$C$50</c:f>
+              <c:f>'Burn down chart'!$C$38:$C$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3980,16 +4049,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1084384</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>330851</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>21167</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1836858</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>76201</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>126592</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>97367</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4284,8 +4353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G117"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.83203125" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -4325,7 +4394,7 @@
         <v>70</v>
       </c>
       <c r="C3" s="3">
-        <v>63</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
@@ -4600,7 +4669,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C34" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.4">
@@ -4628,97 +4697,157 @@
       <c r="A38" s="1">
         <v>20</v>
       </c>
+      <c r="B38" s="1">
+        <v>31</v>
+      </c>
+      <c r="C38" s="1">
+        <v>31</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A39" s="1">
         <v>19</v>
       </c>
+      <c r="C39" s="1">
+        <v>34</v>
+      </c>
       <c r="D39" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A40" s="1">
         <v>18</v>
       </c>
+      <c r="C40" s="1">
+        <v>34</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A41" s="1">
         <v>17</v>
       </c>
+      <c r="C41" s="1">
+        <v>33</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A42" s="1">
         <v>16</v>
       </c>
+      <c r="C42" s="1">
+        <v>32</v>
+      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A43" s="1">
         <v>15</v>
       </c>
+      <c r="B43" s="1">
+        <v>20</v>
+      </c>
+      <c r="C43" s="1">
+        <v>30</v>
+      </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A44" s="1">
         <v>14</v>
       </c>
+      <c r="C44" s="1">
+        <v>30</v>
+      </c>
       <c r="D44" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A45" s="1">
         <v>13</v>
       </c>
+      <c r="C45" s="1">
+        <v>27</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A46" s="1">
         <v>12</v>
       </c>
+      <c r="C46" s="1">
+        <v>22</v>
+      </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A47" s="1">
         <v>11</v>
       </c>
+      <c r="C47" s="1">
+        <v>20</v>
+      </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A48" s="1">
         <v>10</v>
       </c>
+      <c r="B48" s="1">
+        <v>10</v>
+      </c>
+      <c r="C48" s="1">
+        <v>20</v>
+      </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A49" s="1">
         <v>9</v>
       </c>
+      <c r="C49" s="1">
+        <v>19</v>
+      </c>
       <c r="D49" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A50" s="1">
         <v>8</v>
       </c>
+      <c r="C50" s="1">
+        <v>14</v>
+      </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A51" s="1">
         <v>7</v>
       </c>
+      <c r="C51" s="1">
+        <v>14</v>
+      </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A52" s="1">
         <v>6</v>
       </c>
+      <c r="C52" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A53" s="1">
         <v>5</v>
       </c>
+      <c r="B53" s="1">
+        <v>5</v>
+      </c>
+      <c r="C53" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A54" s="1">
         <v>4</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.4">

</xml_diff>